<commit_message>
added sc4.html & sc4.xlsx
</commit_message>
<xml_diff>
--- a/Excel/preferences.xlsx
+++ b/Excel/preferences.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Websites\audacity-mr\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="168">
   <si>
     <t>English</t>
   </si>
@@ -271,24 +276,6 @@
     <t>If you run the installer but do not choose "Reset Preferences" (or say "No" when the "Reset Audacity Preferences" dialog appears), Audacity's installation files will be updated with correct copies but the Audacity settings will remain as before.</t>
   </si>
   <si>
-    <t>प्राधान्ये - धैर्य मॅन्युअल</t>
-  </si>
-  <si>
-    <t>प्राधान्ये</t>
-  </si>
-  <si>
-    <t>ऑडसिटी डेव्हलपमेंट मॅन्युअल वरुन</t>
-  </si>
-  <si>
-    <t>येथे जा: सुचालन, शोध</t>
-  </si>
-  <si>
-    <t>प्राधान्ये आपल्याला ऑडसिटीचे बहुतेक डीफॉल्ट आचरण बदलू देतात.</t>
-  </si>
-  <si>
-    <t>संपादन मेनूचा वापर करून (किंवा शॉर्टकट Ctrl + P वापरुन) पसंती संवादात प्रवेश करता येतो. मॅकवर, प्राधान्ये ऑडसिटी मेनू is +, अंतर्गत असतात.</t>
-  </si>
-  <si>
     <t>सामग्री</t>
   </si>
   <si>
@@ -304,9 +291,6 @@
     <t>प्राधान्ये रीसेट करत आहे</t>
   </si>
   <si>
-    <t>प्राधान्ये संवाद 17 विभागात विभागले गेले आहेत. प्रत्येक विभागाचे वर्णन पृष्ठ (खालील दुव्यांद्वारे प्रवेश केलेले) त्या विभागासाठी डीफॉल्ट पसंती सेटिंग्जची प्रतिमा दर्शविते.</t>
-  </si>
-  <si>
     <t>विभाग</t>
   </si>
   <si>
@@ -328,9 +312,6 @@
     <t>मुद्रित करणे</t>
   </si>
   <si>
-    <t>प्लेथ्रू, विलंब, ध्वनी सक्रिय रेकॉर्डिंग आणि नवीन रेकॉर्ड केलेल्या ट्रॅकचे नाव देण्याची सेटिंग्ज.</t>
-  </si>
-  <si>
     <t>मिडी उपकरणे</t>
   </si>
   <si>
@@ -502,26 +483,64 @@
     <t>अनुप्रयोग डेटासाठी ऑडॅसिटीच्या फोल्डरमध्ये ऑडॅसिटी.एफएफ सेटिंग्ज सेटिंग्ज हटवून ऑडॅसिटी रीस्टार्ट करून आपण फॅक्टरी डीफॉल्टवर प्राधान्ये रीसेट करू शकता. Windows वर, आपण प्रतिष्ठापन दरम्यान "प्राधान्ये रीसेट करा" बॉक्स निवडल्याची खात्री करुन ऑडसिटी पुन्हा स्थापित देखील करू शकता.</t>
   </si>
   <si>
-    <t>विंडोज इंस्टॉलरचा वापर करून प्राधान्ये रीसेट करा</t>
-  </si>
-  <si>
-    <t>Https://web.audacityteam.org/download/windows वरून EXE इंस्टॉलर चालवा.</t>
-  </si>
-  <si>
-    <t>"अतिरिक्त कार्ये निवडा" स्क्रीनवर नेव्हिगेट करा नंतर "प्राधान्ये रीसेट करा" बॉक्समध्ये चेकमार्क लावा आणि स्थापना पूर्ण करा.</t>
-  </si>
-  <si>
-    <t>ऑडीसिटी लाँच करा नंतर "ऑडॅटीस प्राधान्ये रीसेट करा" संवादात होय निवडा.</t>
-  </si>
-  <si>
-    <t>आपण इन्स्टॉलर चालवत असल्यास परंतु "रीसेट प्राधान्ये" न निवडल्यास (किंवा "रीसेट ऑडसेट प्राधान्ये" संवाद दिल्यास "नाही" म्हणाल तर) ऑडिटीच्या इन्स्टॉलेशन फाइल्स योग्य प्रतीसह अद्ययावत केल्या जातील परंतु ऑडसिटी सेटिंग्ज पूर्वीप्रमाणेच राहतील.</t>
+    <t>प्राध्यान्ये - ओड्यासिटी माहितीपुस्तिका</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ओड्यासिटी विकास माहितीपुस्तिकेकडून </t>
+  </si>
+  <si>
+    <t>प्राध्यान्ये</t>
+  </si>
+  <si>
+    <t>येथे जा: निर्देशक ,शोधा</t>
+  </si>
+  <si>
+    <t>प्राधान्ये आपल्याला ओड्यासिटी बहुतेक पूर्वनिर्धारित वर्तन बदलू देतात.</t>
+  </si>
+  <si>
+    <t>पोर्टेबल समायोजन</t>
+  </si>
+  <si>
+    <t>प्राधान्ये पूर्वनिर्धारित करत आहे</t>
+  </si>
+  <si>
+    <r>
+      <t>प्राधान्ये संवाद १७ विभागांमध्ये विभागले गेले आहेत.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> प्रत्येक विभागाचे वर्णन पृष्ठ (खालील दुव्यांद्वारे प्रवेश केलेले) त्या विभागासाठी पूर्वनिर्धारित पसंती समायोजनची प्रतिमा दर्शविते.</t>
+    </r>
+  </si>
+  <si>
+    <t>धवनीमुद्रण यजमान ,पुनर्ध्वनीमुद्रण आणि ध्वनीमुद्रण साधने आणि ध्वनीमुद्रण वाहिनी निवडा.</t>
+  </si>
+  <si>
+    <t>आपण इंस्टॉलर चालवत असल्यास परंतु "पूर्वनिर्धारित प्राधान्ये" न निवडल्यास (किंवा "पूर्वनिर्धारित करा ओड्यासिटी प्राधान्ये" संवाद आढळल्यास "नाही" म्हणाल तर) ओड्यासिटीची स्थापना धारिका योग्य प्रतींसह अद्ययावत केल्या जातील परंतु ओड्यासिटी समायोजन पूर्वीप्रमाणेच राहतील.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ओड्यासिटी उघडा नंतर "पूर्वनिर्धारित करा ओड्यासिटी प्राधान्ये" संवादात, निवडा </t>
+  </si>
+  <si>
+    <t>"अतिरिक्त कार्ये निवडा" पटलावर नेव्हिगेट करा नंतर "प्राधान्ये पूर्वनिर्धारित करा" बॉक्समध्ये चेकमार्क लावा आणि स्थापना पूर्ण करा.</t>
+  </si>
+  <si>
+    <t>विंडोज इंस्टॉलरचा वापर करून प्राधान्ये पूर्वनिर्धारित करा</t>
+  </si>
+  <si>
+    <t>येथून EXE इंस्टॉलर चालवा</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,6 +555,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -573,17 +598,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -630,7 +664,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -662,9 +696,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,6 +731,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -871,14 +907,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="141.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,73 +928,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -960,10 +1002,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -971,10 +1013,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -982,32 +1024,32 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1015,21 +1057,21 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1037,10 +1079,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1048,10 +1090,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1059,10 +1101,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1070,10 +1112,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1081,10 +1123,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1092,10 +1134,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1103,21 +1145,21 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="C22" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1125,10 +1167,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1136,10 +1178,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1147,10 +1189,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1158,10 +1200,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1169,10 +1211,10 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1180,10 +1222,10 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1191,10 +1233,10 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1202,10 +1244,10 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1213,10 +1255,10 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1224,10 +1266,10 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1235,10 +1277,10 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1246,10 +1288,10 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1257,10 +1299,10 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1268,10 +1310,10 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1279,10 +1321,10 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1290,10 +1332,10 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1301,10 +1343,10 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1312,10 +1354,10 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1323,10 +1365,10 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1334,10 +1376,10 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1345,10 +1387,10 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1356,10 +1398,10 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1367,10 +1409,10 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1378,10 +1420,10 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1389,10 +1431,10 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1400,10 +1442,10 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1411,10 +1453,10 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1422,10 +1464,10 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1433,10 +1475,10 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1444,10 +1486,10 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1455,10 +1497,10 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1466,10 +1508,10 @@
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1477,10 +1519,10 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1488,10 +1530,10 @@
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1499,10 +1541,10 @@
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1510,10 +1552,10 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1521,10 +1563,10 @@
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1532,10 +1574,10 @@
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1543,10 +1585,10 @@
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1554,10 +1596,10 @@
         <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1565,10 +1607,10 @@
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1576,10 +1618,10 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1587,10 +1629,10 @@
         <v>11</v>
       </c>
       <c r="C65" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1598,10 +1640,10 @@
         <v>63</v>
       </c>
       <c r="C66" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1609,10 +1651,10 @@
         <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1620,10 +1662,10 @@
         <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1631,10 +1673,10 @@
         <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1642,10 +1684,10 @@
         <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1653,10 +1695,10 @@
         <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1664,10 +1706,10 @@
         <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1675,10 +1717,10 @@
         <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1686,10 +1728,10 @@
         <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1697,10 +1739,10 @@
         <v>72</v>
       </c>
       <c r="C75" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1708,10 +1750,10 @@
         <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1719,10 +1761,10 @@
         <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1730,10 +1772,10 @@
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1741,10 +1783,10 @@
         <v>76</v>
       </c>
       <c r="C79" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1752,10 +1794,10 @@
         <v>77</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1763,10 +1805,10 @@
         <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1774,10 +1816,10 @@
         <v>78</v>
       </c>
       <c r="C82" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1785,65 +1827,66 @@
         <v>79</v>
       </c>
       <c r="C83" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
         <v>80</v>
       </c>
-      <c r="C84" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="C84" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
         <v>81</v>
       </c>
-      <c r="C85" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="C85" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
         <v>82</v>
       </c>
-      <c r="C86" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="C86" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
         <v>83</v>
       </c>
-      <c r="C87" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="C87" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
         <v>84</v>
       </c>
-      <c r="C88" t="s">
-        <v>166</v>
+      <c r="C88" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>